<commit_message>
added 07_x_other_petroleum_products to residential
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\Outlook9th_EBT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362D6575-DC2C-4CC4-99CA-ADA2D41D74AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0071F896-BD64-4630-B6B0-891B022C7D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
+    <workbookView xWindow="-14235" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
   <sheets>
     <sheet name="fuels_by_sectors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="87">
   <si>
     <t>FUELS</t>
   </si>
@@ -727,18 +727,18 @@
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.81640625" customWidth="1"/>
-    <col min="2" max="9" width="13.26953125" customWidth="1"/>
-    <col min="12" max="12" width="23.90625" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="9" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -799,7 +799,7 @@
         <v>Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>9</v>
@@ -829,7 +829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -888,7 +888,7 @@
         <v>01_coal</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -937,7 +937,7 @@
         <v>01_01_coking_coal</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -988,7 +988,7 @@
         <v>01_05_lignite</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>01_x_thermal_coal</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>02_coal_products</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>03_peat</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>04_peat_products</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>06_crude_oil_and_ngl</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>06_01_crude_oil</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>06_02_natural_gas_liquids</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2419,7 +2419,9 @@
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>18</v>
@@ -2441,7 +2443,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>07_x_other_petroleum_products</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="4"/>
@@ -2464,7 +2466,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2523,7 +2525,7 @@
         <v>08_gas</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2578,7 +2580,7 @@
         <v>08_01_natural_gas</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2625,7 +2627,7 @@
         <v>08_02_lng</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2672,7 +2674,7 @@
         <v>08_03_gas_works_gas</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2719,7 +2721,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2766,7 +2768,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2819,7 +2821,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2872,7 +2874,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -2966,7 +2968,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -3015,7 +3017,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -3062,7 +3064,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -3119,7 +3121,7 @@
         <v>15_solid_biomass</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -3168,7 +3170,7 @@
         <v>15_01_fuelwood_and_woodwaste</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>15_02_bagasse</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -3268,7 +3270,7 @@
         <v>15_03_charcoal</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -3315,7 +3317,7 @@
         <v>15_04_black_liquor</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -3364,7 +3366,7 @@
         <v>15_05_other_biomass</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>16_others</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -3476,7 +3478,7 @@
         <v>16_01_biogas</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -3527,7 +3529,7 @@
         <v>16_02_industrial_waste</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -3578,7 +3580,7 @@
         <v>16_03_municipal_solid_waste_renewable</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -3629,7 +3631,7 @@
         <v>16_04_municipal_solid_waste_nonrenewable</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -3682,7 +3684,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>75</v>
       </c>
@@ -3735,7 +3737,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -3883,7 +3885,7 @@
         <v>16_09_other_sources</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -3936,7 +3938,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -4022,7 +4024,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -4078,7 +4080,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -4190,7 +4192,7 @@
         <v>19_total</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -4251,7 +4253,7 @@
         <v>20_total_renewables</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
giving all 16_others subfuels to buildings sector
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD643F-63AA-4287-A6EB-C87E08DC75F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C76E437-3CDF-4F48-8DFC-16D15B8B6143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="87">
   <si>
     <t>FUELS</t>
   </si>
@@ -728,7 +728,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,7 +3488,9 @@
         <v>18</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
         <v>18</v>
@@ -3508,7 +3510,7 @@
       </c>
       <c r="M55" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_02_industrial_waste</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="12"/>
@@ -3539,7 +3541,9 @@
         <v>18</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>18</v>
@@ -3559,7 +3563,7 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_03_municipal_solid_waste_renewable</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="12"/>
@@ -3590,7 +3594,9 @@
         <v>18</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
         <v>18</v>
@@ -3610,7 +3616,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_04_municipal_solid_waste_nonrenewable</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="12"/>
@@ -3643,7 +3649,9 @@
       <c r="C58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
         <v>18</v>
@@ -3663,7 +3671,7 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_05_biogasoline</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="12"/>
@@ -3696,7 +3704,9 @@
       <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
         <v>18</v>
@@ -3716,7 +3726,7 @@
       </c>
       <c r="M59" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_06_biodiesel</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="12"/>
@@ -3747,7 +3757,9 @@
       <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
@@ -3764,7 +3776,7 @@
       </c>
       <c r="M60" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_07_bio_jet_kerosene</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="12"/>
@@ -3795,7 +3807,9 @@
         <v>18</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -3813,7 +3827,7 @@
       </c>
       <c r="M61" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_08_other_liquid_biofuels</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="12"/>
@@ -3844,7 +3858,9 @@
         <v>18</v>
       </c>
       <c r="C62" s="2"/>
-      <c r="D62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3864,7 +3880,7 @@
       </c>
       <c r="M62" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_09_other_sources</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="12"/>
@@ -3897,7 +3913,9 @@
       <c r="C63" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>18</v>
       </c>
@@ -3917,7 +3935,7 @@
       </c>
       <c r="M63" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_x_ammonia</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="12"/>
@@ -4005,7 +4023,9 @@
       <c r="C65" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -4017,7 +4037,7 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>16_x_efuel</v>
       </c>
       <c r="Q65" t="str">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
splitting '08_gas' and '07_petroleum_products' for pipeline
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A992C20-6D2E-456F-9B11-EB2A13A5CC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325F4845-A77F-4F5E-8EF5-32C3A57CC730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="87">
   <si>
     <t>FUELS</t>
   </si>
@@ -727,8 +727,8 @@
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2908,9 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
@@ -2926,7 +2928,7 @@
       </c>
       <c r="M43" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>12_01_of_which_photovoltaics</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="12"/>
@@ -2955,7 +2957,9 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
@@ -2973,7 +2977,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>12_x_other_solar</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="12"/>
@@ -4381,6 +4385,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033DE4B8CEBD9304286F1E0B7BC383844" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d76399d66d45378b52bd24e5db7672eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa" xmlns:ns3="3042e625-934f-4bb2-8533-cbb6446c8b2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e3bb06f6900da50fdd409f0138bcf" ns2:_="" ns3:_="">
     <xsd:import namespace="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
@@ -4591,16 +4604,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA43F71-C302-40B8-A148-F26BCA219CFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B566DB4-C485-4D42-9094-B1E2943EFED1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4617,12 +4629,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA43F71-C302-40B8-A148-F26BCA219CFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
efuel added to hydrogen sector
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DBA64B-10DF-4D69-99FB-5289E86A780D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F36E9E-61E3-4508-A134-7478206503B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="88">
   <si>
     <t>FUELS</t>
   </si>
@@ -730,8 +730,8 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2530,7 @@
         <v>08_gas</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" ref="N35:N64" si="12">IF(OR(E35="a",E35="?"),$A35,"")</f>
+        <f t="shared" ref="N35:N65" si="12">IF(OR(E35="a",E35="?"),$A35,"")</f>
         <v>08_gas</v>
       </c>
       <c r="O35" t="str">
@@ -4069,7 +4069,9 @@
       <c r="D65" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -4080,6 +4082,10 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="11"/>
+        <v>16_x_efuel</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="12"/>
         <v>16_x_efuel</v>
       </c>
       <c r="Q65" t="str">

</xml_diff>

<commit_message>
a little bit of modification to the TPES calculation
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F36E9E-61E3-4508-A134-7478206503B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E0BCB0-EEBF-4210-AF29-1E1BB293B380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
@@ -730,8 +730,8 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S66" sqref="S66"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added more fuels to transport sector
</commit_message>
<xml_diff>
--- a/config/fuels_used_by_modellers.xlsx
+++ b/config/fuels_used_by_modellers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB4B545-E588-4517-8014-66812DE4E869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77598BE6-F0CD-4998-B422-723B249A279A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{4DA73B7A-5DB8-461F-82E0-D287C45E52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="90">
   <si>
     <t>FUELS</t>
   </si>
@@ -736,8 +736,8 @@
   <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,9 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1031,7 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>01_x_thermal_coal</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="3"/>
@@ -4482,15 +4484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033DE4B8CEBD9304286F1E0B7BC383844" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d76399d66d45378b52bd24e5db7672eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa" xmlns:ns3="3042e625-934f-4bb2-8533-cbb6446c8b2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e3bb06f6900da50fdd409f0138bcf" ns2:_="" ns3:_="">
     <xsd:import namespace="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
@@ -4701,15 +4694,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA43F71-C302-40B8-A148-F26BCA219CFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B566DB4-C485-4D42-9094-B1E2943EFED1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4726,4 +4720,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AA43F71-C302-40B8-A148-F26BCA219CFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>